<commit_message>
he arreglat els coms
</commit_message>
<xml_diff>
--- a/ph_distr_direct_40deg.xlsx
+++ b/ph_distr_direct_40deg.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,15 +443,799 @@
         <v>-487.5</v>
       </c>
       <c r="B2" t="n">
-        <v>-120.7894970314423</v>
+        <v>53.53996495497859</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
+        <v>-477.6515151515151</v>
+      </c>
+      <c r="B3" t="n">
+        <v>55.26933905388023</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>-467.8030303030303</v>
+      </c>
+      <c r="B4" t="n">
+        <v>56.99871315278187</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>-457.9545454545454</v>
+      </c>
+      <c r="B5" t="n">
+        <v>58.72808725168352</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>-448.1060606060606</v>
+      </c>
+      <c r="B6" t="n">
+        <v>60.45746135058516</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>-438.2575757575758</v>
+      </c>
+      <c r="B7" t="n">
+        <v>62.18683544948692</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>-428.4090909090909</v>
+      </c>
+      <c r="B8" t="n">
+        <v>63.91620954838845</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>-418.5606060606061</v>
+      </c>
+      <c r="B9" t="n">
+        <v>65.6455836472901</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>-408.7121212121212</v>
+      </c>
+      <c r="B10" t="n">
+        <v>67.37495774619174</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>-398.8636363636364</v>
+      </c>
+      <c r="B11" t="n">
+        <v>69.1043318450935</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>-389.0151515151515</v>
+      </c>
+      <c r="B12" t="n">
+        <v>70.83370594399503</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>-379.1666666666667</v>
+      </c>
+      <c r="B13" t="n">
+        <v>72.56308004289679</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>-369.3181818181818</v>
+      </c>
+      <c r="B14" t="n">
+        <v>74.29245414179832</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>-359.469696969697</v>
+      </c>
+      <c r="B15" t="n">
+        <v>76.02182824070007</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>-349.6212121212121</v>
+      </c>
+      <c r="B16" t="n">
+        <v>77.7512023396016</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>-339.7727272727273</v>
+      </c>
+      <c r="B17" t="n">
+        <v>79.48057643850336</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>-329.9242424242424</v>
+      </c>
+      <c r="B18" t="n">
+        <v>81.20995053740501</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>-320.0757575757576</v>
+      </c>
+      <c r="B19" t="n">
+        <v>82.93932463630665</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>-310.2272727272727</v>
+      </c>
+      <c r="B20" t="n">
+        <v>84.66869873520841</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>-300.3787878787879</v>
+      </c>
+      <c r="B21" t="n">
+        <v>86.39807283411005</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>-290.5303030303031</v>
+      </c>
+      <c r="B22" t="n">
+        <v>88.12744693301158</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>-280.6818181818182</v>
+      </c>
+      <c r="B23" t="n">
+        <v>89.85682103191334</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>-270.8333333333334</v>
+      </c>
+      <c r="B24" t="n">
+        <v>91.58619513081499</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>-260.9848484848485</v>
+      </c>
+      <c r="B25" t="n">
+        <v>93.31556922971663</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>-251.1363636363637</v>
+      </c>
+      <c r="B26" t="n">
+        <v>95.04494332861827</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>-241.2878787878788</v>
+      </c>
+      <c r="B27" t="n">
+        <v>96.77431742751992</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>-231.4393939393939</v>
+      </c>
+      <c r="B28" t="n">
+        <v>98.50369152642156</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>-221.5909090909091</v>
+      </c>
+      <c r="B29" t="n">
+        <v>100.2330656253232</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>-211.7424242424242</v>
+      </c>
+      <c r="B30" t="n">
+        <v>101.9624397242249</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>-201.8939393939394</v>
+      </c>
+      <c r="B31" t="n">
+        <v>103.6918138231265</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>-192.0454545454546</v>
+      </c>
+      <c r="B32" t="n">
+        <v>105.4211879220281</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>-182.1969696969697</v>
+      </c>
+      <c r="B33" t="n">
+        <v>107.1505620209298</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>-172.3484848484849</v>
+      </c>
+      <c r="B34" t="n">
+        <v>108.8799361198314</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>-162.5</v>
+      </c>
+      <c r="B35" t="n">
+        <v>110.6093102187331</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>-152.6515151515152</v>
+      </c>
+      <c r="B36" t="n">
+        <v>112.3386843176347</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>-142.8030303030303</v>
+      </c>
+      <c r="B37" t="n">
+        <v>114.0680584165364</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>-132.9545454545455</v>
+      </c>
+      <c r="B38" t="n">
+        <v>115.797432515438</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>-123.1060606060606</v>
+      </c>
+      <c r="B39" t="n">
+        <v>117.5268066143396</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>-113.2575757575758</v>
+      </c>
+      <c r="B40" t="n">
+        <v>119.2561807132413</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>-103.4090909090909</v>
+      </c>
+      <c r="B41" t="n">
+        <v>120.9855548121431</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>-93.56060606060612</v>
+      </c>
+      <c r="B42" t="n">
+        <v>122.7149289110446</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>-83.71212121212125</v>
+      </c>
+      <c r="B43" t="n">
+        <v>124.4443030099463</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>-73.86363636363637</v>
+      </c>
+      <c r="B44" t="n">
+        <v>126.173677108848</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>-64.01515151515156</v>
+      </c>
+      <c r="B45" t="n">
+        <v>127.9030512077496</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>-54.16666666666669</v>
+      </c>
+      <c r="B46" t="n">
+        <v>129.6324253066513</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>-44.31818181818187</v>
+      </c>
+      <c r="B47" t="n">
+        <v>131.3617994055529</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>-34.469696969697</v>
+      </c>
+      <c r="B48" t="n">
+        <v>133.0911735044546</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>-24.62121212121218</v>
+      </c>
+      <c r="B49" t="n">
+        <v>134.8205476033562</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>-14.77272727272731</v>
+      </c>
+      <c r="B50" t="n">
+        <v>136.5499217022579</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>-4.924242424242436</v>
+      </c>
+      <c r="B51" t="n">
+        <v>138.2792958011595</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>4.924242424242379</v>
+      </c>
+      <c r="B52" t="n">
+        <v>140.0086699000612</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>14.77272727272725</v>
+      </c>
+      <c r="B53" t="n">
+        <v>141.7380439989629</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>24.62121212121212</v>
+      </c>
+      <c r="B54" t="n">
+        <v>143.4674180978645</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>34.46969696969688</v>
+      </c>
+      <c r="B55" t="n">
+        <v>145.1967921967662</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>44.31818181818176</v>
+      </c>
+      <c r="B56" t="n">
+        <v>146.9261662956678</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>54.16666666666663</v>
+      </c>
+      <c r="B57" t="n">
+        <v>148.6555403945694</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>64.0151515151515</v>
+      </c>
+      <c r="B58" t="n">
+        <v>150.3849144934711</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>73.86363636363637</v>
+      </c>
+      <c r="B59" t="n">
+        <v>152.1142885923727</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>83.71212121212113</v>
+      </c>
+      <c r="B60" t="n">
+        <v>153.8436626912744</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>93.56060606060601</v>
+      </c>
+      <c r="B61" t="n">
+        <v>155.573036790176</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>103.4090909090909</v>
+      </c>
+      <c r="B62" t="n">
+        <v>157.3024108890777</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>113.2575757575758</v>
+      </c>
+      <c r="B63" t="n">
+        <v>159.0317849879794</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>123.1060606060605</v>
+      </c>
+      <c r="B64" t="n">
+        <v>160.761159086881</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>132.9545454545454</v>
+      </c>
+      <c r="B65" t="n">
+        <v>162.4905331857827</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>142.8030303030303</v>
+      </c>
+      <c r="B66" t="n">
+        <v>164.2199072846843</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>152.6515151515151</v>
+      </c>
+      <c r="B67" t="n">
+        <v>165.949281383586</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>162.5</v>
+      </c>
+      <c r="B68" t="n">
+        <v>167.6786554824876</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>172.3484848484848</v>
+      </c>
+      <c r="B69" t="n">
+        <v>169.4080295813893</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>182.1969696969696</v>
+      </c>
+      <c r="B70" t="n">
+        <v>171.1374036802909</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>192.0454545454545</v>
+      </c>
+      <c r="B71" t="n">
+        <v>172.8667777791926</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>201.8939393939394</v>
+      </c>
+      <c r="B72" t="n">
+        <v>174.5961518780942</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>211.7424242424241</v>
+      </c>
+      <c r="B73" t="n">
+        <v>176.3255259769959</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>221.590909090909</v>
+      </c>
+      <c r="B74" t="n">
+        <v>178.0549000758975</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>231.4393939393939</v>
+      </c>
+      <c r="B75" t="n">
+        <v>179.7842741747992</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>241.2878787878788</v>
+      </c>
+      <c r="B76" t="n">
+        <v>181.5136482737008</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>251.1363636363636</v>
+      </c>
+      <c r="B77" t="n">
+        <v>183.2430223726025</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>260.9848484848484</v>
+      </c>
+      <c r="B78" t="n">
+        <v>184.9723964715041</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>270.8333333333333</v>
+      </c>
+      <c r="B79" t="n">
+        <v>186.7017705704058</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>280.6818181818181</v>
+      </c>
+      <c r="B80" t="n">
+        <v>188.4311446693074</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>290.530303030303</v>
+      </c>
+      <c r="B81" t="n">
+        <v>190.1605187682091</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>300.3787878787878</v>
+      </c>
+      <c r="B82" t="n">
+        <v>191.8898928671107</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>310.2272727272726</v>
+      </c>
+      <c r="B83" t="n">
+        <v>193.6192669660124</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>320.0757575757575</v>
+      </c>
+      <c r="B84" t="n">
+        <v>195.348641064914</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>329.9242424242424</v>
+      </c>
+      <c r="B85" t="n">
+        <v>197.0780151638157</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>339.7727272727273</v>
+      </c>
+      <c r="B86" t="n">
+        <v>198.8073892627174</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>349.621212121212</v>
+      </c>
+      <c r="B87" t="n">
+        <v>200.5367633616189</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>359.4696969696969</v>
+      </c>
+      <c r="B88" t="n">
+        <v>202.2661374605206</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>369.3181818181818</v>
+      </c>
+      <c r="B89" t="n">
+        <v>203.9955115594223</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>379.1666666666666</v>
+      </c>
+      <c r="B90" t="n">
+        <v>205.7248856583239</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>389.0151515151515</v>
+      </c>
+      <c r="B91" t="n">
+        <v>207.4542597572256</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>398.8636363636363</v>
+      </c>
+      <c r="B92" t="n">
+        <v>209.1836338561272</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>408.7121212121211</v>
+      </c>
+      <c r="B93" t="n">
+        <v>210.9130079550289</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>418.560606060606</v>
+      </c>
+      <c r="B94" t="n">
+        <v>212.6423820539305</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>428.4090909090909</v>
+      </c>
+      <c r="B95" t="n">
+        <v>214.3717561528322</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>438.2575757575756</v>
+      </c>
+      <c r="B96" t="n">
+        <v>216.1011302517338</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>448.1060606060605</v>
+      </c>
+      <c r="B97" t="n">
+        <v>217.8305043506355</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>457.9545454545454</v>
+      </c>
+      <c r="B98" t="n">
+        <v>219.5598784495371</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>467.8030303030303</v>
+      </c>
+      <c r="B99" t="n">
+        <v>221.2892525484388</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>477.6515151515151</v>
+      </c>
+      <c r="B100" t="n">
+        <v>223.0186266473405</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
         <v>487.5</v>
       </c>
-      <c r="B3" t="n">
-        <v>49.84801594469673</v>
+      <c r="B101" t="n">
+        <v>224.7480007462421</v>
       </c>
     </row>
   </sheetData>

</xml_diff>